<commit_message>
Updating STM32 Hero Board BSP with documentation and examples (Work In Progress)
</commit_message>
<xml_diff>
--- a/boards/arm/stm32/piconomix_hero_board/px_board_gpio.xlsx
+++ b/boards/arm/stm32/piconomix_hero_board/px_board_gpio.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BCA34A-656F-4A9D-A195-57ED3D076933}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GPIO" sheetId="7" r:id="rId1"/>
@@ -19,11 +20,12 @@
     <definedName name="OutputType">Options!$C$2:$C$4</definedName>
     <definedName name="Pull">Options!$G$2:$G$4</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -156,9 +158,6 @@
     <t>PX_GPIO_UART2_RX</t>
   </si>
   <si>
-    <t>PX_GPIO_DAC</t>
-  </si>
-  <si>
     <t>PX_GPIO_ADC2</t>
   </si>
   <si>
@@ -219,9 +218,6 @@
     <t>PX_GPIO_LCD_RS</t>
   </si>
   <si>
-    <t>PX_GPIO_SPI2_CS_DF</t>
-  </si>
-  <si>
     <t>PX_GPIO_SPI2_SCK</t>
   </si>
   <si>
@@ -264,12 +260,6 @@
     <t>PX_GPIO_LCD_BTN_6_YES</t>
   </si>
   <si>
-    <t>PX_GPIO_UART3_TX</t>
-  </si>
-  <si>
-    <t>PX_GPIO_UART3_RX</t>
-  </si>
-  <si>
     <t>PX_GPIO_LCD_BTN_4_DN</t>
   </si>
   <si>
@@ -403,12 +393,24 @@
   </si>
   <si>
     <t>#define GPIOH_MODER_VAL \</t>
+  </si>
+  <si>
+    <t>PX_GPIO_UART4_TX</t>
+  </si>
+  <si>
+    <t>PX_GPIO_UART4_RX</t>
+  </si>
+  <si>
+    <t>PX_GPIO_DAC1</t>
+  </si>
+  <si>
+    <t>PX_GPIO_SPI2_CS_SF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -561,28 +563,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1071,6 +1073,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1106,6 +1125,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1281,7 +1317,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC0A020"/>
   </sheetPr>
@@ -1361,28 +1397,28 @@
       <c r="O1" s="1"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -1473,7 +1509,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -1731,7 +1767,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>122</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
@@ -1784,40 +1820,40 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>#define PX_GPIO_DAC PX_GPIO(A, 4, PX_GPIO_MODE_ANA, PX_GPIO_OTYPE_NA, PX_GPIO_OSPEED_NA, PX_GPIO_PULL_NO, PX_GPIO_OUT_INIT_NA, PX_GPIO_AF_NA)</v>
+        <v>#define PX_GPIO_DAC1 PX_GPIO(A, 4, PX_GPIO_MODE_ANA, PX_GPIO_OTYPE_NA, PX_GPIO_OSPEED_NA, PX_GPIO_PULL_NO, PX_GPIO_OUT_INIT_NA, PX_GPIO_AF_NA)</v>
       </c>
       <c r="S6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>static const px_gpio_handle_t px_gpio_dac = {PX_GPIO_DAC};</v>
+        <v>static const px_gpio_handle_t px_gpio_dac1 = {PX_GPIO_DAC1};</v>
       </c>
       <c r="U6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_DAC) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_DAC1) \</v>
       </c>
       <c r="W6" s="3" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_DAC) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_DAC1) \</v>
       </c>
       <c r="Y6" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_DAC) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_DAC1) \</v>
       </c>
       <c r="AA6" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_DAC) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_DAC1) \</v>
       </c>
       <c r="AC6" s="3" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_DAC) \</v>
+        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_DAC1) \</v>
       </c>
       <c r="AE6" s="3" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_DAC) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_DAC1) \</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
@@ -1903,7 +1939,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>12</v>
@@ -2075,7 +2111,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>12</v>
@@ -2161,7 +2197,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>12</v>
@@ -2247,7 +2283,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>12</v>
@@ -2333,7 +2369,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
@@ -2419,7 +2455,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>12</v>
@@ -2505,7 +2541,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>12</v>
@@ -2591,7 +2627,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>12</v>
@@ -2677,7 +2713,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
@@ -2779,30 +2815,30 @@
       <c r="O18" s="10"/>
       <c r="P18" s="2"/>
       <c r="U18" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="AE18" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="4">
         <v>0</v>
@@ -2885,10 +2921,10 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="4">
         <v>1</v>
@@ -2971,10 +3007,10 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="4">
         <v>2</v>
@@ -3024,43 +3060,43 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>#define PX_GPIO_SPI2_CS_DF PX_GPIO(B, 2, PX_GPIO_MODE_OUT, PX_GPIO_OTYPE_PP, PX_GPIO_OSPEED_LO, PX_GPIO_PULL_NO, PX_GPIO_OUT_INIT_HI, PX_GPIO_AF_NA)</v>
+        <v>#define PX_GPIO_SPI2_CS_SF PX_GPIO(B, 2, PX_GPIO_MODE_OUT, PX_GPIO_OTYPE_PP, PX_GPIO_OSPEED_LO, PX_GPIO_PULL_NO, PX_GPIO_OUT_INIT_HI, PX_GPIO_AF_NA)</v>
       </c>
       <c r="S21" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>static const px_gpio_handle_t px_gpio_spi2_cs_df = {PX_GPIO_SPI2_CS_DF};</v>
+        <v>static const px_gpio_handle_t px_gpio_spi2_cs_sf = {PX_GPIO_SPI2_CS_SF};</v>
       </c>
       <c r="U21" s="3" t="str">
         <f t="shared" ref="U21:U33" si="13">CONCATENATE("    + PX_GPIO_REG_MODER_INIT(",$A21,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SPI2_CS_DF) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SPI2_CS_SF) \</v>
       </c>
       <c r="W21" s="3" t="str">
         <f t="shared" ref="W21:W33" si="14">CONCATENATE("    + PX_GPIO_REG_OTYPER_INIT(",$A21,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SPI2_CS_DF) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SPI2_CS_SF) \</v>
       </c>
       <c r="Y21" s="3" t="str">
         <f t="shared" ref="Y21:Y33" si="15">CONCATENATE("    + PX_GPIO_REG_OSPEEDR_INIT(",$A21,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SPI2_CS_DF) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SPI2_CS_SF) \</v>
       </c>
       <c r="AA21" s="3" t="str">
         <f t="shared" ref="AA21:AA33" si="16">CONCATENATE("    + PX_GPIO_REG_PUPDR_INIT(",$A21,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SPI2_CS_DF) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SPI2_CS_SF) \</v>
       </c>
       <c r="AC21" s="3" t="str">
         <f t="shared" ref="AC21:AC33" si="17">CONCATENATE("  + PX_GPIO_REG_ODR_INIT(",$A21,") \")</f>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SPI2_CS_DF) \</v>
+        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SPI2_CS_SF) \</v>
       </c>
       <c r="AE21" s="3" t="str">
         <f t="shared" ref="AE21:AE26" si="18">CONCATENATE("    + PX_GPIO_REG_AFRL_INIT(",$A21,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_SPI2_CS_DF) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_SPI2_CS_SF) \</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="4">
         <v>3</v>
@@ -3143,10 +3179,10 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="4">
         <v>4</v>
@@ -3229,10 +3265,10 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="4">
         <v>5</v>
@@ -3315,10 +3351,10 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="4">
         <v>6</v>
@@ -3401,10 +3437,10 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="4">
         <v>7</v>
@@ -3487,10 +3523,10 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="4">
         <v>8</v>
@@ -3573,10 +3609,10 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="4">
         <v>9</v>
@@ -3659,10 +3695,10 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" s="4">
         <v>10</v>
@@ -3745,10 +3781,10 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="4">
         <v>11</v>
@@ -3831,10 +3867,10 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" s="4">
         <v>12</v>
@@ -3917,10 +3953,10 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" s="4">
         <v>13</v>
@@ -4003,10 +4039,10 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="4">
         <v>14</v>
@@ -4033,11 +4069,11 @@
         <v>1</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K33" s="7">
         <f>VLOOKUP(J33,Options!G$2:H$100,2,FALSE)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>25</v>
@@ -4056,7 +4092,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>#define PX_GPIO_SPI2_MISO PX_GPIO(B, 14, PX_GPIO_MODE_AF, PX_GPIO_OTYPE_NA, PX_GPIO_OSPEED_NA, PX_GPIO_PULL_NO, PX_GPIO_OUT_INIT_NA, PX_GPIO_AF_0)</v>
+        <v>#define PX_GPIO_SPI2_MISO PX_GPIO(B, 14, PX_GPIO_MODE_AF, PX_GPIO_OTYPE_NA, PX_GPIO_OSPEED_NA, PX_GPIO_PULL_DN, PX_GPIO_OUT_INIT_NA, PX_GPIO_AF_0)</v>
       </c>
       <c r="S33" s="3" t="str">
         <f t="shared" si="1"/>
@@ -4089,10 +4125,10 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="4">
         <v>15</v>
@@ -4191,30 +4227,30 @@
       <c r="O35" s="10"/>
       <c r="P35" s="2"/>
       <c r="U35" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="AA35" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="AC35" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AE35" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C36" s="4">
         <v>0</v>
@@ -4297,10 +4333,10 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C37" s="4">
         <v>1</v>
@@ -4383,10 +4419,10 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C38" s="4">
         <v>2</v>
@@ -4469,10 +4505,10 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C39" s="4">
         <v>3</v>
@@ -4555,10 +4591,10 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C40" s="4">
         <v>4</v>
@@ -4641,10 +4677,10 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C41" s="4">
         <v>5</v>
@@ -4727,10 +4763,10 @@
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C42" s="4">
         <v>6</v>
@@ -4813,10 +4849,10 @@
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C43" s="4">
         <v>7</v>
@@ -4899,10 +4935,10 @@
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C44" s="4">
         <v>8</v>
@@ -4985,10 +5021,10 @@
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C45" s="4">
         <v>9</v>
@@ -5071,10 +5107,10 @@
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C46" s="4">
         <v>10</v>
@@ -5115,52 +5151,52 @@
         <v>3</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="O46" s="7">
         <f>VLOOKUP(N46,Options!K$2:L$100,2,FALSE)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="P46" s="2"/>
       <c r="Q46" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>#define PX_GPIO_UART3_TX PX_GPIO(C, 10, PX_GPIO_MODE_AF, PX_GPIO_OTYPE_PP, PX_GPIO_OSPEED_LO, PX_GPIO_PULL_NO, PX_GPIO_OUT_INIT_HI, PX_GPIO_AF_4)</v>
+        <v>#define PX_GPIO_UART4_TX PX_GPIO(C, 10, PX_GPIO_MODE_AF, PX_GPIO_OTYPE_PP, PX_GPIO_OSPEED_LO, PX_GPIO_PULL_NO, PX_GPIO_OUT_INIT_HI, PX_GPIO_AF_6)</v>
       </c>
       <c r="S46" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>static const px_gpio_handle_t px_gpio_uart3_tx = {PX_GPIO_UART3_TX};</v>
+        <v>static const px_gpio_handle_t px_gpio_uart4_tx = {PX_GPIO_UART4_TX};</v>
       </c>
       <c r="U46" s="3" t="str">
         <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_UART3_TX) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_UART4_TX) \</v>
       </c>
       <c r="W46" s="3" t="str">
         <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_UART3_TX) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_UART4_TX) \</v>
       </c>
       <c r="Y46" s="3" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_UART3_TX) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_UART4_TX) \</v>
       </c>
       <c r="AA46" s="3" t="str">
         <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_UART3_TX) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_UART4_TX) \</v>
       </c>
       <c r="AC46" s="3" t="str">
         <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_UART3_TX) \</v>
+        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_UART4_TX) \</v>
       </c>
       <c r="AE46" s="3" t="str">
         <f t="shared" ref="AE46:AE50" si="30">CONCATENATE("    + PX_GPIO_REG_AFRH_INIT(",$A46,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_UART3_TX) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_UART4_TX) \</v>
       </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C47" s="4">
         <v>11</v>
@@ -5201,52 +5237,52 @@
         <v>1</v>
       </c>
       <c r="N47" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="O47" s="7">
         <f>VLOOKUP(N47,Options!K$2:L$100,2,FALSE)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="P47" s="2"/>
       <c r="Q47" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>#define PX_GPIO_UART3_RX PX_GPIO(C, 11, PX_GPIO_MODE_AF, PX_GPIO_OTYPE_NA, PX_GPIO_OSPEED_LO, PX_GPIO_PULL_UP, PX_GPIO_OUT_INIT_NA, PX_GPIO_AF_4)</v>
+        <v>#define PX_GPIO_UART4_RX PX_GPIO(C, 11, PX_GPIO_MODE_AF, PX_GPIO_OTYPE_NA, PX_GPIO_OSPEED_LO, PX_GPIO_PULL_UP, PX_GPIO_OUT_INIT_NA, PX_GPIO_AF_6)</v>
       </c>
       <c r="S47" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>static const px_gpio_handle_t px_gpio_uart3_rx = {PX_GPIO_UART3_RX};</v>
+        <v>static const px_gpio_handle_t px_gpio_uart4_rx = {PX_GPIO_UART4_RX};</v>
       </c>
       <c r="U47" s="3" t="str">
         <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_UART3_RX) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_UART4_RX) \</v>
       </c>
       <c r="W47" s="3" t="str">
         <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_UART3_RX) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_UART4_RX) \</v>
       </c>
       <c r="Y47" s="3" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_UART3_RX) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_UART4_RX) \</v>
       </c>
       <c r="AA47" s="3" t="str">
         <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_UART3_RX) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_UART4_RX) \</v>
       </c>
       <c r="AC47" s="3" t="str">
         <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_UART3_RX) \</v>
+        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_UART4_RX) \</v>
       </c>
       <c r="AE47" s="3" t="str">
         <f t="shared" si="30"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_UART3_RX) \</v>
+        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_UART4_RX) \</v>
       </c>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C48" s="4">
         <v>12</v>
@@ -5329,10 +5365,10 @@
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C49" s="4">
         <v>13</v>
@@ -5415,10 +5451,10 @@
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C50" s="4">
         <v>14</v>
@@ -5501,10 +5537,10 @@
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C51" s="4">
         <v>15</v>
@@ -5603,30 +5639,30 @@
       <c r="O52" s="10"/>
       <c r="P52" s="2"/>
       <c r="U52" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="W52" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="Y52" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="AA52" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AC52" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="AE52" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C53" s="4">
         <v>2</v>
@@ -5725,30 +5761,30 @@
       <c r="O54" s="10"/>
       <c r="P54" s="2"/>
       <c r="U54" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="W54" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="Y54" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="AA54" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="AC54" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AE54" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C55" s="4">
         <v>0</v>
@@ -5831,10 +5867,10 @@
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C56" s="4">
         <v>1</v>
@@ -6120,22 +6156,22 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D56" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Mode</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F56" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>OutputType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H56" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>OutputSpeed</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J56" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>Pull</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L56" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>OutputInit</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N56" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>AltFn</formula1>
     </dataValidation>
   </dataValidations>
@@ -6145,7 +6181,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Added px_dbg_board_disable() and px_board_stop_mode()
</commit_message>
<xml_diff>
--- a/boards/arm/stm32/piconomix_hero_board/px_board_gpio.xlsx
+++ b/boards/arm/stm32/piconomix_hero_board/px_board_gpio.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BCA34A-656F-4A9D-A195-57ED3D076933}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433321B4-00CC-414E-BBC2-FFC14730EBB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3453,18 +3453,18 @@
         <v>1</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G26" s="7">
         <f>VLOOKUP(F26,Options!C$2:D$100,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I26" s="7">
         <f>VLOOKUP(H26,Options!E$2:F$100,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>6</v>
@@ -3490,7 +3490,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>#define PX_GPIO_7_SD_CD PX_GPIO(B, 7, PX_GPIO_MODE_IN, PX_GPIO_OTYPE_PP, PX_GPIO_OSPEED_LO, PX_GPIO_PULL_UP, PX_GPIO_OUT_INIT_NA, PX_GPIO_AF_NA)</v>
+        <v>#define PX_GPIO_7_SD_CD PX_GPIO(B, 7, PX_GPIO_MODE_IN, PX_GPIO_OTYPE_NA, PX_GPIO_OSPEED_NA, PX_GPIO_PULL_UP, PX_GPIO_OUT_INIT_NA, PX_GPIO_AF_NA)</v>
       </c>
       <c r="S26" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3553,11 +3553,11 @@
         <v>2</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="K27" s="7">
         <f>VLOOKUP(J27,Options!G$2:H$100,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>27</v>
@@ -3576,7 +3576,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>#define PX_GPIO_I2C1_SCL PX_GPIO(B, 8, PX_GPIO_MODE_AF, PX_GPIO_OTYPE_OD, PX_GPIO_OSPEED_LO, PX_GPIO_PULL_NO, PX_GPIO_OUT_INIT_HI, PX_GPIO_AF_4)</v>
+        <v>#define PX_GPIO_I2C1_SCL PX_GPIO(B, 8, PX_GPIO_MODE_AF, PX_GPIO_OTYPE_OD, PX_GPIO_OSPEED_LO, PX_GPIO_PULL_UP, PX_GPIO_OUT_INIT_HI, PX_GPIO_AF_4)</v>
       </c>
       <c r="S27" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3639,11 +3639,11 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="K28" s="7">
         <f>VLOOKUP(J28,Options!G$2:H$100,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>27</v>
@@ -3662,7 +3662,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>#define PX_GPIO_I2C1_SDA PX_GPIO(B, 9, PX_GPIO_MODE_AF, PX_GPIO_OTYPE_OD, PX_GPIO_OSPEED_LO, PX_GPIO_PULL_NO, PX_GPIO_OUT_INIT_HI, PX_GPIO_AF_4)</v>
+        <v>#define PX_GPIO_I2C1_SDA PX_GPIO(B, 9, PX_GPIO_MODE_AF, PX_GPIO_OTYPE_OD, PX_GPIO_OSPEED_LO, PX_GPIO_PULL_UP, PX_GPIO_OUT_INIT_HI, PX_GPIO_AF_4)</v>
       </c>
       <c r="S28" s="3" t="str">
         <f t="shared" si="1"/>
@@ -4772,11 +4772,11 @@
         <v>6</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E42" s="7">
         <f>VLOOKUP(D42,Options!A$2:B$100,2,FALSE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>16</v>
@@ -4816,7 +4816,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>#define PX_GPIO_PWM_BUZZER PX_GPIO(C, 6, PX_GPIO_MODE_AF, PX_GPIO_OTYPE_PP, PX_GPIO_OSPEED_HI, PX_GPIO_PULL_NO, PX_GPIO_OUT_INIT_NA, PX_GPIO_AF_2)</v>
+        <v>#define PX_GPIO_PWM_BUZZER PX_GPIO(C, 6, PX_GPIO_MODE_ANA, PX_GPIO_OTYPE_PP, PX_GPIO_OSPEED_HI, PX_GPIO_PULL_NO, PX_GPIO_OUT_INIT_NA, PX_GPIO_AF_2)</v>
       </c>
       <c r="S42" s="3" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Added px_gpio_init_stm32l072rb.h to simplify initialization of GPIO ports with px_gpio_port_init()
</commit_message>
<xml_diff>
--- a/boards/arm/stm32/piconomix_hero_board/px_board_gpio.xlsx
+++ b/boards/arm/stm32/piconomix_hero_board/px_board_gpio.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433321B4-00CC-414E-BBC2-FFC14730EBB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33E35F9-4F07-4B3A-A4B4-28180AA923CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="95">
   <si>
     <t>Mode</t>
   </si>
@@ -305,96 +305,6 @@
     <t>Global variables</t>
   </si>
   <si>
-    <t>#define GPIOA_PUPDR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOB_PUPDR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOC_PUPDR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOD_PUPDR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOH_PUPDR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOA_OTYPER_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOB_OTYPER_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOC_OTYPER_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOD_OTYPER_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOH_OTYPER_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOA_OSPEEDR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOB_OSPEEDR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOC_OSPEEDR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOD_OSPEEDR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOH_OSPEEDR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOA_ODR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOB_ODR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOC_ODR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOD_ODR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOH_ODR_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOA_AFRL_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOB_AFRL_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOC_AFRL_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOD_AFRL_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOH_AFRL_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOA_MODER_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOB_MODER_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOC_MODER_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOD_MODER_VAL \</t>
-  </si>
-  <si>
-    <t>#define GPIOH_MODER_VAL \</t>
-  </si>
-  <si>
     <t>PX_GPIO_UART4_TX</t>
   </si>
   <si>
@@ -405,6 +315,9 @@
   </si>
   <si>
     <t>PX_GPIO_SPI2_CS_SF</t>
+  </si>
+  <si>
+    <t>Map</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1234,7 @@
   <sheetPr>
     <tabColor rgb="FFC0A020"/>
   </sheetPr>
-  <dimension ref="A1:AE57"/>
+  <dimension ref="A1:U57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1347,21 +1260,11 @@
     <col min="18" max="18" width="9.140625" style="3"/>
     <col min="19" max="19" width="62.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.140625" style="3"/>
-    <col min="21" max="21" width="44.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="3"/>
-    <col min="23" max="23" width="45.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="3"/>
-    <col min="25" max="25" width="46.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" style="3"/>
-    <col min="27" max="27" width="44.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="3"/>
-    <col min="29" max="29" width="41.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.140625" style="3"/>
-    <col min="31" max="31" width="41.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="3"/>
+    <col min="21" max="21" width="62.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1403,25 +1306,10 @@
         <v>89</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
@@ -1483,31 +1371,11 @@
         <v>static const px_gpio_handle_t px_gpio_3 = {PX_GPIO_3};</v>
       </c>
       <c r="U2" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_MODER_INIT(",$A2,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_MODER_INIT(PX_GPIO_3) \</v>
-      </c>
-      <c r="W2" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_OTYPER_INIT(",$A2,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_OTYPER_INIT(PX_GPIO_3) \</v>
-      </c>
-      <c r="Y2" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_OSPEEDR_INIT(",$A2,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_3) \</v>
-      </c>
-      <c r="AA2" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_PUPDR_INIT(",$A2,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_PUPDR_INIT(PX_GPIO_3) \</v>
-      </c>
-      <c r="AC2" s="3" t="str">
-        <f>CONCATENATE("    PX_GPIO_REG_ODR_INIT(",$A2,") \")</f>
-        <v xml:space="preserve">    PX_GPIO_REG_ODR_INIT(PX_GPIO_3) \</v>
-      </c>
-      <c r="AE2" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_AFRL_INIT(",$A2,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_AFRL_INIT(PX_GPIO_3) \</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+        <f>CONCATENATE("#define PX_GPIO_",$B2,$C2," ",$A2)</f>
+        <v>#define PX_GPIO_A0 PX_GPIO_3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>70</v>
       </c>
@@ -1569,31 +1437,11 @@
         <v>static const px_gpio_handle_t px_gpio_2 = {PX_GPIO_2};</v>
       </c>
       <c r="U3" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_MODER_INIT(",$A3,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_2) \</v>
-      </c>
-      <c r="W3" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_OTYPER_INIT(",$A3,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_2) \</v>
-      </c>
-      <c r="Y3" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_OSPEEDR_INIT(",$A3,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_2) \</v>
-      </c>
-      <c r="AA3" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_PUPDR_INIT(",$A3,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_2) \</v>
-      </c>
-      <c r="AC3" s="3" t="str">
-        <f>CONCATENATE("  + PX_GPIO_REG_ODR_INIT(",$A3,") \")</f>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_2) \</v>
-      </c>
-      <c r="AE3" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_AFRL_INIT(",$A3,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_2) \</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" ref="U3:U55" si="2">CONCATENATE("#define PX_GPIO_",$B3,$C3," ",$A3)</f>
+        <v>#define PX_GPIO_A1 PX_GPIO_2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
@@ -1655,31 +1503,11 @@
         <v>static const px_gpio_handle_t px_gpio_uart2_tx = {PX_GPIO_UART2_TX};</v>
       </c>
       <c r="U4" s="3" t="str">
-        <f t="shared" ref="U4:U16" si="2">CONCATENATE("    + PX_GPIO_REG_MODER_INIT(",$A4,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_UART2_TX) \</v>
-      </c>
-      <c r="W4" s="3" t="str">
-        <f t="shared" ref="W4:W16" si="3">CONCATENATE("    + PX_GPIO_REG_OTYPER_INIT(",$A4,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_UART2_TX) \</v>
-      </c>
-      <c r="Y4" s="3" t="str">
-        <f t="shared" ref="Y4:Y16" si="4">CONCATENATE("    + PX_GPIO_REG_OSPEEDR_INIT(",$A4,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_UART2_TX) \</v>
-      </c>
-      <c r="AA4" s="3" t="str">
-        <f t="shared" ref="AA4:AA16" si="5">CONCATENATE("    + PX_GPIO_REG_PUPDR_INIT(",$A4,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_UART2_TX) \</v>
-      </c>
-      <c r="AC4" s="3" t="str">
-        <f t="shared" ref="AC4:AC16" si="6">CONCATENATE("  + PX_GPIO_REG_ODR_INIT(",$A4,") \")</f>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_UART2_TX) \</v>
-      </c>
-      <c r="AE4" s="3" t="str">
-        <f t="shared" ref="AE4:AE9" si="7">CONCATENATE("    + PX_GPIO_REG_AFRL_INIT(",$A4,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_UART2_TX) \</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_A2 PX_GPIO_UART2_TX</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
@@ -1742,32 +1570,12 @@
       </c>
       <c r="U5" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_UART2_RX) \</v>
-      </c>
-      <c r="W5" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_UART2_RX) \</v>
-      </c>
-      <c r="Y5" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_UART2_RX) \</v>
-      </c>
-      <c r="AA5" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_UART2_RX) \</v>
-      </c>
-      <c r="AC5" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_UART2_RX) \</v>
-      </c>
-      <c r="AE5" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_UART2_RX) \</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_A3 PX_GPIO_UART2_RX</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
@@ -1828,30 +1636,10 @@
       </c>
       <c r="U6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_DAC1) \</v>
-      </c>
-      <c r="W6" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_DAC1) \</v>
-      </c>
-      <c r="Y6" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_DAC1) \</v>
-      </c>
-      <c r="AA6" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_DAC1) \</v>
-      </c>
-      <c r="AC6" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_DAC1) \</v>
-      </c>
-      <c r="AE6" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_DAC1) \</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_A4 PX_GPIO_DAC1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
@@ -1914,30 +1702,10 @@
       </c>
       <c r="U7" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_1) \</v>
-      </c>
-      <c r="W7" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_1) \</v>
-      </c>
-      <c r="Y7" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_1) \</v>
-      </c>
-      <c r="AA7" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_1) \</v>
-      </c>
-      <c r="AC7" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_1) \</v>
-      </c>
-      <c r="AE7" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_1) \</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_A5 PX_GPIO_1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>53</v>
       </c>
@@ -2000,30 +1768,10 @@
       </c>
       <c r="U8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_0) \</v>
-      </c>
-      <c r="W8" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_0) \</v>
-      </c>
-      <c r="Y8" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_0) \</v>
-      </c>
-      <c r="AA8" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_0) \</v>
-      </c>
-      <c r="AC8" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_0) \</v>
-      </c>
-      <c r="AE8" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_0) \</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_A6 PX_GPIO_0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
@@ -2086,30 +1834,10 @@
       </c>
       <c r="U9" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_ADC3) \</v>
-      </c>
-      <c r="W9" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_ADC3) \</v>
-      </c>
-      <c r="Y9" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_ADC3) \</v>
-      </c>
-      <c r="AA9" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_ADC3) \</v>
-      </c>
-      <c r="AC9" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_ADC3) \</v>
-      </c>
-      <c r="AE9" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_ADC3) \</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_A7 PX_GPIO_ADC3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>43</v>
       </c>
@@ -2172,30 +1900,10 @@
       </c>
       <c r="U10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_USB_DET) \</v>
-      </c>
-      <c r="W10" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_USB_DET) \</v>
-      </c>
-      <c r="Y10" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_USB_DET) \</v>
-      </c>
-      <c r="AA10" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_USB_DET) \</v>
-      </c>
-      <c r="AC10" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_USB_DET) \</v>
-      </c>
-      <c r="AE10" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_AFRH_INIT(",$A10,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_AFRH_INIT(PX_GPIO_USB_DET) \</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_A8 PX_GPIO_USB_DET</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
@@ -2258,30 +1966,10 @@
       </c>
       <c r="U11" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_UART1_TX) \</v>
-      </c>
-      <c r="W11" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_UART1_TX) \</v>
-      </c>
-      <c r="Y11" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_UART1_TX) \</v>
-      </c>
-      <c r="AA11" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_UART1_TX) \</v>
-      </c>
-      <c r="AC11" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_UART1_TX) \</v>
-      </c>
-      <c r="AE11" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_AFRH_INIT(",$A11,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_UART1_TX) \</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_A9 PX_GPIO_UART1_TX</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
@@ -2344,30 +2032,10 @@
       </c>
       <c r="U12" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_UART1_RX) \</v>
-      </c>
-      <c r="W12" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_UART1_RX) \</v>
-      </c>
-      <c r="Y12" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_UART1_RX) \</v>
-      </c>
-      <c r="AA12" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_UART1_RX) \</v>
-      </c>
-      <c r="AC12" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_UART1_RX) \</v>
-      </c>
-      <c r="AE12" s="3" t="str">
-        <f t="shared" ref="AE12:AE16" si="8">CONCATENATE("    + PX_GPIO_REG_AFRH_INIT(",$A12,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_UART1_RX) \</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_A10 PX_GPIO_UART1_RX</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
@@ -2430,30 +2098,10 @@
       </c>
       <c r="U13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_USB1D_N) \</v>
-      </c>
-      <c r="W13" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_USB1D_N) \</v>
-      </c>
-      <c r="Y13" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_USB1D_N) \</v>
-      </c>
-      <c r="AA13" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_USB1D_N) \</v>
-      </c>
-      <c r="AC13" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_USB1D_N) \</v>
-      </c>
-      <c r="AE13" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_USB1D_N) \</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_A11 PX_GPIO_USB1D_N</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>47</v>
       </c>
@@ -2516,30 +2164,10 @@
       </c>
       <c r="U14" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_USB1D_P) \</v>
-      </c>
-      <c r="W14" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_USB1D_P) \</v>
-      </c>
-      <c r="Y14" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_USB1D_P) \</v>
-      </c>
-      <c r="AA14" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_USB1D_P) \</v>
-      </c>
-      <c r="AC14" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_USB1D_P) \</v>
-      </c>
-      <c r="AE14" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_USB1D_P) \</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_A12 PX_GPIO_USB1D_P</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>48</v>
       </c>
@@ -2602,30 +2230,10 @@
       </c>
       <c r="U15" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SWDIO) \</v>
-      </c>
-      <c r="W15" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SWDIO) \</v>
-      </c>
-      <c r="Y15" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SWDIO) \</v>
-      </c>
-      <c r="AA15" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SWDIO) \</v>
-      </c>
-      <c r="AC15" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SWDIO) \</v>
-      </c>
-      <c r="AE15" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_SWDIO) \</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_A13 PX_GPIO_SWDIO</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>49</v>
       </c>
@@ -2688,30 +2296,10 @@
       </c>
       <c r="U16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SWDCK) \</v>
-      </c>
-      <c r="W16" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SWDCK) \</v>
-      </c>
-      <c r="Y16" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SWDCK) \</v>
-      </c>
-      <c r="AA16" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SWDCK) \</v>
-      </c>
-      <c r="AC16" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SWDCK) \</v>
-      </c>
-      <c r="AE16" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_SWDCK) \</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_A14 PX_GPIO_SWDCK</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>50</v>
       </c>
@@ -2773,31 +2361,11 @@
         <v>static const px_gpio_handle_t px_gpio_lcd_btn_5_no = {PX_GPIO_LCD_BTN_5_NO};</v>
       </c>
       <c r="U17" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_MODER_INIT(",$A17,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_LCD_BTN_5_NO)</v>
-      </c>
-      <c r="W17" s="3" t="str">
-        <f t="shared" ref="W17" si="9">CONCATENATE("    + PX_GPIO_REG_OTYPER_INIT(",$A17,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_LCD_BTN_5_NO)</v>
-      </c>
-      <c r="Y17" s="3" t="str">
-        <f t="shared" ref="Y17" si="10">CONCATENATE("    + PX_GPIO_REG_OSPEEDR_INIT(",$A17,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_LCD_BTN_5_NO)</v>
-      </c>
-      <c r="AA17" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_PUPDR_INIT(",$A17,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_LCD_BTN_5_NO)</v>
-      </c>
-      <c r="AC17" s="3" t="str">
-        <f t="shared" ref="AC17" si="11">CONCATENATE("  + PX_GPIO_REG_ODR_INIT(",$A17,")")</f>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_LCD_BTN_5_NO)</v>
-      </c>
-      <c r="AE17" s="3" t="str">
-        <f t="shared" ref="AE17" si="12">CONCATENATE("    + PX_GPIO_REG_AFRH_INIT(",$A17,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_LCD_BTN_5_NO)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_A15 PX_GPIO_LCD_BTN_5_NO</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -2814,26 +2382,8 @@
       <c r="N18" s="9"/>
       <c r="O18" s="10"/>
       <c r="P18" s="2"/>
-      <c r="U18" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC18" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE18" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>84</v>
       </c>
@@ -2895,31 +2445,11 @@
         <v>static const px_gpio_handle_t px_gpio_adc0 = {PX_GPIO_ADC0};</v>
       </c>
       <c r="U19" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_MODER_INIT(",$A19,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_MODER_INIT(PX_GPIO_ADC0) \</v>
-      </c>
-      <c r="W19" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_OTYPER_INIT(",$A19,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_OTYPER_INIT(PX_GPIO_ADC0) \</v>
-      </c>
-      <c r="Y19" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_OSPEEDR_INIT(",$A19,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_ADC0) \</v>
-      </c>
-      <c r="AA19" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_PUPDR_INIT(",$A19,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_PUPDR_INIT(PX_GPIO_ADC0) \</v>
-      </c>
-      <c r="AC19" s="3" t="str">
-        <f>CONCATENATE("    PX_GPIO_REG_ODR_INIT(",$A19,") \")</f>
-        <v xml:space="preserve">    PX_GPIO_REG_ODR_INIT(PX_GPIO_ADC0) \</v>
-      </c>
-      <c r="AE19" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_AFRL_INIT(",$A19,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_AFRL_INIT(PX_GPIO_ADC0) \</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B0 PX_GPIO_ADC0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>69</v>
       </c>
@@ -2981,33 +2511,13 @@
         <v>static const px_gpio_handle_t px_gpio_adc_vbat = {PX_GPIO_ADC_VBAT};</v>
       </c>
       <c r="U20" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_MODER_INIT(",$A20,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_ADC_VBAT) \</v>
-      </c>
-      <c r="W20" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_OTYPER_INIT(",$A20,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_ADC_VBAT) \</v>
-      </c>
-      <c r="Y20" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_OSPEEDR_INIT(",$A20,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_ADC_VBAT) \</v>
-      </c>
-      <c r="AA20" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_PUPDR_INIT(",$A20,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_ADC_VBAT) \</v>
-      </c>
-      <c r="AC20" s="3" t="str">
-        <f>CONCATENATE("  + PX_GPIO_REG_ODR_INIT(",$A20,") \")</f>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_ADC_VBAT) \</v>
-      </c>
-      <c r="AE20" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_AFRL_INIT(",$A20,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_ADC_VBAT) \</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B1 PX_GPIO_ADC_VBAT</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>52</v>
@@ -3067,31 +2577,11 @@
         <v>static const px_gpio_handle_t px_gpio_spi2_cs_sf = {PX_GPIO_SPI2_CS_SF};</v>
       </c>
       <c r="U21" s="3" t="str">
-        <f t="shared" ref="U21:U33" si="13">CONCATENATE("    + PX_GPIO_REG_MODER_INIT(",$A21,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SPI2_CS_SF) \</v>
-      </c>
-      <c r="W21" s="3" t="str">
-        <f t="shared" ref="W21:W33" si="14">CONCATENATE("    + PX_GPIO_REG_OTYPER_INIT(",$A21,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SPI2_CS_SF) \</v>
-      </c>
-      <c r="Y21" s="3" t="str">
-        <f t="shared" ref="Y21:Y33" si="15">CONCATENATE("    + PX_GPIO_REG_OSPEEDR_INIT(",$A21,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SPI2_CS_SF) \</v>
-      </c>
-      <c r="AA21" s="3" t="str">
-        <f t="shared" ref="AA21:AA33" si="16">CONCATENATE("    + PX_GPIO_REG_PUPDR_INIT(",$A21,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SPI2_CS_SF) \</v>
-      </c>
-      <c r="AC21" s="3" t="str">
-        <f t="shared" ref="AC21:AC33" si="17">CONCATENATE("  + PX_GPIO_REG_ODR_INIT(",$A21,") \")</f>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SPI2_CS_SF) \</v>
-      </c>
-      <c r="AE21" s="3" t="str">
-        <f t="shared" ref="AE21:AE26" si="18">CONCATENATE("    + PX_GPIO_REG_AFRL_INIT(",$A21,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_SPI2_CS_SF) \</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B2 PX_GPIO_SPI2_CS_SF</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>55</v>
       </c>
@@ -3153,31 +2643,11 @@
         <v>static const px_gpio_handle_t px_gpio_spi1_sck = {PX_GPIO_SPI1_SCK};</v>
       </c>
       <c r="U22" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SPI1_SCK) \</v>
-      </c>
-      <c r="W22" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SPI1_SCK) \</v>
-      </c>
-      <c r="Y22" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SPI1_SCK) \</v>
-      </c>
-      <c r="AA22" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SPI1_SCK) \</v>
-      </c>
-      <c r="AC22" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SPI1_SCK) \</v>
-      </c>
-      <c r="AE22" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_SPI1_SCK) \</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B3 PX_GPIO_SPI1_SCK</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
@@ -3239,31 +2709,11 @@
         <v>static const px_gpio_handle_t px_gpio_spi1_miso = {PX_GPIO_SPI1_MISO};</v>
       </c>
       <c r="U23" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SPI1_MISO) \</v>
-      </c>
-      <c r="W23" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SPI1_MISO) \</v>
-      </c>
-      <c r="Y23" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SPI1_MISO) \</v>
-      </c>
-      <c r="AA23" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SPI1_MISO) \</v>
-      </c>
-      <c r="AC23" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SPI1_MISO) \</v>
-      </c>
-      <c r="AE23" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_SPI1_MISO) \</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B4 PX_GPIO_SPI1_MISO</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>57</v>
       </c>
@@ -3325,31 +2775,11 @@
         <v>static const px_gpio_handle_t px_gpio_spi1_mosi = {PX_GPIO_SPI1_MOSI};</v>
       </c>
       <c r="U24" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SPI1_MOSI) \</v>
-      </c>
-      <c r="W24" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SPI1_MOSI) \</v>
-      </c>
-      <c r="Y24" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SPI1_MOSI) \</v>
-      </c>
-      <c r="AA24" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SPI1_MOSI) \</v>
-      </c>
-      <c r="AC24" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SPI1_MOSI) \</v>
-      </c>
-      <c r="AE24" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_SPI1_MOSI) \</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B5 PX_GPIO_SPI1_MOSI</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>85</v>
       </c>
@@ -3411,31 +2841,11 @@
         <v>static const px_gpio_handle_t px_gpio_spi1_cs = {PX_GPIO_SPI1_CS};</v>
       </c>
       <c r="U25" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SPI1_CS) \</v>
-      </c>
-      <c r="W25" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SPI1_CS) \</v>
-      </c>
-      <c r="Y25" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SPI1_CS) \</v>
-      </c>
-      <c r="AA25" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SPI1_CS) \</v>
-      </c>
-      <c r="AC25" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SPI1_CS) \</v>
-      </c>
-      <c r="AE25" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_SPI1_CS) \</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B6 PX_GPIO_SPI1_CS</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>86</v>
       </c>
@@ -3497,31 +2907,11 @@
         <v>static const px_gpio_handle_t px_gpio_7_sd_cd = {PX_GPIO_7_SD_CD};</v>
       </c>
       <c r="U26" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_7_SD_CD) \</v>
-      </c>
-      <c r="W26" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_7_SD_CD) \</v>
-      </c>
-      <c r="Y26" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_7_SD_CD) \</v>
-      </c>
-      <c r="AA26" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_7_SD_CD) \</v>
-      </c>
-      <c r="AC26" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_7_SD_CD) \</v>
-      </c>
-      <c r="AE26" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_7_SD_CD) \</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B7 PX_GPIO_7_SD_CD</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>58</v>
       </c>
@@ -3583,31 +2973,11 @@
         <v>static const px_gpio_handle_t px_gpio_i2c1_scl = {PX_GPIO_I2C1_SCL};</v>
       </c>
       <c r="U27" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_I2C1_SCL) \</v>
-      </c>
-      <c r="W27" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_I2C1_SCL) \</v>
-      </c>
-      <c r="Y27" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_I2C1_SCL) \</v>
-      </c>
-      <c r="AA27" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_I2C1_SCL) \</v>
-      </c>
-      <c r="AC27" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_I2C1_SCL) \</v>
-      </c>
-      <c r="AE27" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_AFRH_INIT(",$A27,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_AFRH_INIT(PX_GPIO_I2C1_SCL) \</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B8 PX_GPIO_I2C1_SCL</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>59</v>
       </c>
@@ -3669,31 +3039,11 @@
         <v>static const px_gpio_handle_t px_gpio_i2c1_sda = {PX_GPIO_I2C1_SDA};</v>
       </c>
       <c r="U28" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_I2C1_SDA) \</v>
-      </c>
-      <c r="W28" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_I2C1_SDA) \</v>
-      </c>
-      <c r="Y28" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_I2C1_SDA) \</v>
-      </c>
-      <c r="AA28" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_I2C1_SDA) \</v>
-      </c>
-      <c r="AC28" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_I2C1_SDA) \</v>
-      </c>
-      <c r="AE28" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_AFRH_INIT(",$A28,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_I2C1_SDA) \</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B9 PX_GPIO_I2C1_SDA</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>54</v>
       </c>
@@ -3755,31 +3105,11 @@
         <v>static const px_gpio_handle_t px_gpio_spi2_cs_lcd = {PX_GPIO_SPI2_CS_LCD};</v>
       </c>
       <c r="U29" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SPI2_CS_LCD) \</v>
-      </c>
-      <c r="W29" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SPI2_CS_LCD) \</v>
-      </c>
-      <c r="Y29" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SPI2_CS_LCD) \</v>
-      </c>
-      <c r="AA29" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SPI2_CS_LCD) \</v>
-      </c>
-      <c r="AC29" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SPI2_CS_LCD) \</v>
-      </c>
-      <c r="AE29" s="3" t="str">
-        <f t="shared" ref="AE29:AE33" si="19">CONCATENATE("    + PX_GPIO_REG_AFRH_INIT(",$A29,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_SPI2_CS_LCD) \</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B10 PX_GPIO_SPI2_CS_LCD</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>60</v>
       </c>
@@ -3841,31 +3171,11 @@
         <v>static const px_gpio_handle_t px_gpio_lcd_rs = {PX_GPIO_LCD_RS};</v>
       </c>
       <c r="U30" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_LCD_RS) \</v>
-      </c>
-      <c r="W30" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_LCD_RS) \</v>
-      </c>
-      <c r="Y30" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_LCD_RS) \</v>
-      </c>
-      <c r="AA30" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_LCD_RS) \</v>
-      </c>
-      <c r="AC30" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_LCD_RS) \</v>
-      </c>
-      <c r="AE30" s="3" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_LCD_RS) \</v>
-      </c>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B11 PX_GPIO_LCD_RS</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>87</v>
       </c>
@@ -3927,31 +3237,11 @@
         <v>static const px_gpio_handle_t px_gpio_lcd_backlight = {PX_GPIO_LCD_BACKLIGHT};</v>
       </c>
       <c r="U31" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_LCD_BACKLIGHT) \</v>
-      </c>
-      <c r="W31" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_LCD_BACKLIGHT) \</v>
-      </c>
-      <c r="Y31" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_LCD_BACKLIGHT) \</v>
-      </c>
-      <c r="AA31" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_LCD_BACKLIGHT) \</v>
-      </c>
-      <c r="AC31" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_LCD_BACKLIGHT) \</v>
-      </c>
-      <c r="AE31" s="3" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_LCD_BACKLIGHT) \</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B12 PX_GPIO_LCD_BACKLIGHT</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>61</v>
       </c>
@@ -4013,31 +3303,11 @@
         <v>static const px_gpio_handle_t px_gpio_spi2_sck = {PX_GPIO_SPI2_SCK};</v>
       </c>
       <c r="U32" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SPI2_SCK) \</v>
-      </c>
-      <c r="W32" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SPI2_SCK) \</v>
-      </c>
-      <c r="Y32" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SPI2_SCK) \</v>
-      </c>
-      <c r="AA32" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SPI2_SCK) \</v>
-      </c>
-      <c r="AC32" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SPI2_SCK) \</v>
-      </c>
-      <c r="AE32" s="3" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_SPI2_SCK) \</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B13 PX_GPIO_SPI2_SCK</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>62</v>
       </c>
@@ -4099,31 +3369,11 @@
         <v>static const px_gpio_handle_t px_gpio_spi2_miso = {PX_GPIO_SPI2_MISO};</v>
       </c>
       <c r="U33" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SPI2_MISO) \</v>
-      </c>
-      <c r="W33" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SPI2_MISO) \</v>
-      </c>
-      <c r="Y33" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SPI2_MISO) \</v>
-      </c>
-      <c r="AA33" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SPI2_MISO) \</v>
-      </c>
-      <c r="AC33" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SPI2_MISO) \</v>
-      </c>
-      <c r="AE33" s="3" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_SPI2_MISO) \</v>
-      </c>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B14 PX_GPIO_SPI2_MISO</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>63</v>
       </c>
@@ -4185,31 +3435,11 @@
         <v>static const px_gpio_handle_t px_gpio_spi2_mosi = {PX_GPIO_SPI2_MOSI};</v>
       </c>
       <c r="U34" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_MODER_INIT(",$A34,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_SPI2_MOSI)</v>
-      </c>
-      <c r="W34" s="3" t="str">
-        <f t="shared" ref="W34" si="20">CONCATENATE("    + PX_GPIO_REG_OTYPER_INIT(",$A34,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SPI2_MOSI)</v>
-      </c>
-      <c r="Y34" s="3" t="str">
-        <f t="shared" ref="Y34" si="21">CONCATENATE("    + PX_GPIO_REG_OSPEEDR_INIT(",$A34,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SPI2_MOSI)</v>
-      </c>
-      <c r="AA34" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_PUPDR_INIT(",$A34,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SPI2_MOSI)</v>
-      </c>
-      <c r="AC34" s="3" t="str">
-        <f t="shared" ref="AC34" si="22">CONCATENATE("  + PX_GPIO_REG_ODR_INIT(",$A34,")")</f>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_SPI2_MOSI)</v>
-      </c>
-      <c r="AE34" s="3" t="str">
-        <f t="shared" ref="AE34" si="23">CONCATENATE("    + PX_GPIO_REG_AFRH_INIT(",$A34,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_SPI2_MOSI)</v>
-      </c>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B15 PX_GPIO_SPI2_MOSI</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -4226,26 +3456,8 @@
       <c r="N35" s="9"/>
       <c r="O35" s="10"/>
       <c r="P35" s="2"/>
-      <c r="U35" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="W35" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y35" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA35" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC35" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE35" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>76</v>
       </c>
@@ -4307,31 +3519,11 @@
         <v>static const px_gpio_handle_t px_gpio_lcd_btn_1_lt = {PX_GPIO_LCD_BTN_1_LT};</v>
       </c>
       <c r="U36" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_MODER_INIT(",$A36,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_MODER_INIT(PX_GPIO_LCD_BTN_1_LT) \</v>
-      </c>
-      <c r="W36" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_OTYPER_INIT(",$A36,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_OTYPER_INIT(PX_GPIO_LCD_BTN_1_LT) \</v>
-      </c>
-      <c r="Y36" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_OSPEEDR_INIT(",$A36,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_LCD_BTN_1_LT) \</v>
-      </c>
-      <c r="AA36" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_PUPDR_INIT(",$A36,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_PUPDR_INIT(PX_GPIO_LCD_BTN_1_LT) \</v>
-      </c>
-      <c r="AC36" s="3" t="str">
-        <f>CONCATENATE("    PX_GPIO_REG_ODR_INIT(",$A36,") \")</f>
-        <v xml:space="preserve">    PX_GPIO_REG_ODR_INIT(PX_GPIO_LCD_BTN_1_LT) \</v>
-      </c>
-      <c r="AE36" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_AFRL_INIT(",$A36,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_AFRL_INIT(PX_GPIO_LCD_BTN_1_LT) \</v>
-      </c>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C0 PX_GPIO_LCD_BTN_1_LT</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>66</v>
       </c>
@@ -4393,31 +3585,11 @@
         <v>static const px_gpio_handle_t px_gpio_6 = {PX_GPIO_6};</v>
       </c>
       <c r="U37" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_MODER_INIT(",$A37,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_6) \</v>
-      </c>
-      <c r="W37" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_OTYPER_INIT(",$A37,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_6) \</v>
-      </c>
-      <c r="Y37" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_OSPEEDR_INIT(",$A37,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_6) \</v>
-      </c>
-      <c r="AA37" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_PUPDR_INIT(",$A37,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_6) \</v>
-      </c>
-      <c r="AC37" s="3" t="str">
-        <f>CONCATENATE("  + PX_GPIO_REG_ODR_INIT(",$A37,") \")</f>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_6) \</v>
-      </c>
-      <c r="AE37" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_AFRL_INIT(",$A37,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_6) \</v>
-      </c>
-    </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C1 PX_GPIO_6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>67</v>
       </c>
@@ -4479,31 +3651,11 @@
         <v>static const px_gpio_handle_t px_gpio_5 = {PX_GPIO_5};</v>
       </c>
       <c r="U38" s="3" t="str">
-        <f t="shared" ref="U38:U50" si="24">CONCATENATE("    + PX_GPIO_REG_MODER_INIT(",$A38,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_5) \</v>
-      </c>
-      <c r="W38" s="3" t="str">
-        <f t="shared" ref="W38:W50" si="25">CONCATENATE("    + PX_GPIO_REG_OTYPER_INIT(",$A38,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_5) \</v>
-      </c>
-      <c r="Y38" s="3" t="str">
-        <f t="shared" ref="Y38:Y50" si="26">CONCATENATE("    + PX_GPIO_REG_OSPEEDR_INIT(",$A38,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_5) \</v>
-      </c>
-      <c r="AA38" s="3" t="str">
-        <f t="shared" ref="AA38:AA50" si="27">CONCATENATE("    + PX_GPIO_REG_PUPDR_INIT(",$A38,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_5) \</v>
-      </c>
-      <c r="AC38" s="3" t="str">
-        <f t="shared" ref="AC38:AC50" si="28">CONCATENATE("  + PX_GPIO_REG_ODR_INIT(",$A38,") \")</f>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_5) \</v>
-      </c>
-      <c r="AE38" s="3" t="str">
-        <f t="shared" ref="AE38:AE43" si="29">CONCATENATE("    + PX_GPIO_REG_AFRL_INIT(",$A38,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_5) \</v>
-      </c>
-    </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C2 PX_GPIO_5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>68</v>
       </c>
@@ -4565,31 +3717,11 @@
         <v>static const px_gpio_handle_t px_gpio_4 = {PX_GPIO_4};</v>
       </c>
       <c r="U39" s="3" t="str">
-        <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_4) \</v>
-      </c>
-      <c r="W39" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_4) \</v>
-      </c>
-      <c r="Y39" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_4) \</v>
-      </c>
-      <c r="AA39" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_4) \</v>
-      </c>
-      <c r="AC39" s="3" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_4) \</v>
-      </c>
-      <c r="AE39" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_4) \</v>
-      </c>
-    </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C3 PX_GPIO_4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>41</v>
       </c>
@@ -4651,31 +3783,11 @@
         <v>static const px_gpio_handle_t px_gpio_adc2 = {PX_GPIO_ADC2};</v>
       </c>
       <c r="U40" s="3" t="str">
-        <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_ADC2) \</v>
-      </c>
-      <c r="W40" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_ADC2) \</v>
-      </c>
-      <c r="Y40" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_ADC2) \</v>
-      </c>
-      <c r="AA40" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_ADC2) \</v>
-      </c>
-      <c r="AC40" s="3" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_ADC2) \</v>
-      </c>
-      <c r="AE40" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_ADC2) \</v>
-      </c>
-    </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C4 PX_GPIO_ADC2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>42</v>
       </c>
@@ -4737,31 +3849,11 @@
         <v>static const px_gpio_handle_t px_gpio_adc1 = {PX_GPIO_ADC1};</v>
       </c>
       <c r="U41" s="3" t="str">
-        <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_ADC1) \</v>
-      </c>
-      <c r="W41" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_ADC1) \</v>
-      </c>
-      <c r="Y41" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_ADC1) \</v>
-      </c>
-      <c r="AA41" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_ADC1) \</v>
-      </c>
-      <c r="AC41" s="3" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_ADC1) \</v>
-      </c>
-      <c r="AE41" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_ADC1) \</v>
-      </c>
-    </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C5 PX_GPIO_ADC1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>71</v>
       </c>
@@ -4823,31 +3915,11 @@
         <v>static const px_gpio_handle_t px_gpio_pwm_buzzer = {PX_GPIO_PWM_BUZZER};</v>
       </c>
       <c r="U42" s="3" t="str">
-        <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_PWM_BUZZER) \</v>
-      </c>
-      <c r="W42" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_PWM_BUZZER) \</v>
-      </c>
-      <c r="Y42" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_PWM_BUZZER) \</v>
-      </c>
-      <c r="AA42" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_PWM_BUZZER) \</v>
-      </c>
-      <c r="AC42" s="3" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_PWM_BUZZER) \</v>
-      </c>
-      <c r="AE42" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_PWM_BUZZER) \</v>
-      </c>
-    </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C6 PX_GPIO_PWM_BUZZER</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>72</v>
       </c>
@@ -4909,31 +3981,11 @@
         <v>static const px_gpio_handle_t px_gpio_vbat_meas_en = {PX_GPIO_VBAT_MEAS_EN};</v>
       </c>
       <c r="U43" s="3" t="str">
-        <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_VBAT_MEAS_EN) \</v>
-      </c>
-      <c r="W43" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_VBAT_MEAS_EN) \</v>
-      </c>
-      <c r="Y43" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_VBAT_MEAS_EN) \</v>
-      </c>
-      <c r="AA43" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_VBAT_MEAS_EN) \</v>
-      </c>
-      <c r="AC43" s="3" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_VBAT_MEAS_EN) \</v>
-      </c>
-      <c r="AE43" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_VBAT_MEAS_EN) \</v>
-      </c>
-    </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C7 PX_GPIO_VBAT_MEAS_EN</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>73</v>
       </c>
@@ -4995,31 +4047,11 @@
         <v>static const px_gpio_handle_t px_gpio_3v3_hold = {PX_GPIO_3V3_HOLD};</v>
       </c>
       <c r="U44" s="3" t="str">
-        <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_3V3_HOLD) \</v>
-      </c>
-      <c r="W44" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_3V3_HOLD) \</v>
-      </c>
-      <c r="Y44" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_3V3_HOLD) \</v>
-      </c>
-      <c r="AA44" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_3V3_HOLD) \</v>
-      </c>
-      <c r="AC44" s="3" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_3V3_HOLD) \</v>
-      </c>
-      <c r="AE44" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_AFRH_INIT(",$A44,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_AFRH_INIT(PX_GPIO_3V3_HOLD) \</v>
-      </c>
-    </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C8 PX_GPIO_3V3_HOLD</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>74</v>
       </c>
@@ -5081,33 +4113,13 @@
         <v>static const px_gpio_handle_t px_gpio_lcd_btn_6_yes = {PX_GPIO_LCD_BTN_6_YES};</v>
       </c>
       <c r="U45" s="3" t="str">
-        <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_LCD_BTN_6_YES) \</v>
-      </c>
-      <c r="W45" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_LCD_BTN_6_YES) \</v>
-      </c>
-      <c r="Y45" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_LCD_BTN_6_YES) \</v>
-      </c>
-      <c r="AA45" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_LCD_BTN_6_YES) \</v>
-      </c>
-      <c r="AC45" s="3" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_LCD_BTN_6_YES) \</v>
-      </c>
-      <c r="AE45" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_AFRH_INIT(",$A45,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_LCD_BTN_6_YES) \</v>
-      </c>
-    </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C9 PX_GPIO_LCD_BTN_6_YES</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>64</v>
@@ -5167,33 +4179,13 @@
         <v>static const px_gpio_handle_t px_gpio_uart4_tx = {PX_GPIO_UART4_TX};</v>
       </c>
       <c r="U46" s="3" t="str">
-        <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_UART4_TX) \</v>
-      </c>
-      <c r="W46" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_UART4_TX) \</v>
-      </c>
-      <c r="Y46" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_UART4_TX) \</v>
-      </c>
-      <c r="AA46" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_UART4_TX) \</v>
-      </c>
-      <c r="AC46" s="3" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_UART4_TX) \</v>
-      </c>
-      <c r="AE46" s="3" t="str">
-        <f t="shared" ref="AE46:AE50" si="30">CONCATENATE("    + PX_GPIO_REG_AFRH_INIT(",$A46,") \")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_UART4_TX) \</v>
-      </c>
-    </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C10 PX_GPIO_UART4_TX</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>64</v>
@@ -5253,31 +4245,11 @@
         <v>static const px_gpio_handle_t px_gpio_uart4_rx = {PX_GPIO_UART4_RX};</v>
       </c>
       <c r="U47" s="3" t="str">
-        <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_UART4_RX) \</v>
-      </c>
-      <c r="W47" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_UART4_RX) \</v>
-      </c>
-      <c r="Y47" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_UART4_RX) \</v>
-      </c>
-      <c r="AA47" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_UART4_RX) \</v>
-      </c>
-      <c r="AC47" s="3" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_UART4_RX) \</v>
-      </c>
-      <c r="AE47" s="3" t="str">
-        <f t="shared" si="30"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_UART4_RX) \</v>
-      </c>
-    </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C11 PX_GPIO_UART4_RX</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>75</v>
       </c>
@@ -5339,31 +4311,11 @@
         <v>static const px_gpio_handle_t px_gpio_lcd_btn_4_dn = {PX_GPIO_LCD_BTN_4_DN};</v>
       </c>
       <c r="U48" s="3" t="str">
-        <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_LCD_BTN_4_DN) \</v>
-      </c>
-      <c r="W48" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_LCD_BTN_4_DN) \</v>
-      </c>
-      <c r="Y48" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_LCD_BTN_4_DN) \</v>
-      </c>
-      <c r="AA48" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_LCD_BTN_4_DN) \</v>
-      </c>
-      <c r="AC48" s="3" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_LCD_BTN_4_DN) \</v>
-      </c>
-      <c r="AE48" s="3" t="str">
-        <f t="shared" si="30"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_LCD_BTN_4_DN) \</v>
-      </c>
-    </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C12 PX_GPIO_LCD_BTN_4_DN</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>83</v>
       </c>
@@ -5425,31 +4377,11 @@
         <v>static const px_gpio_handle_t px_gpio_lcd_btn_3_up = {PX_GPIO_LCD_BTN_3_UP};</v>
       </c>
       <c r="U49" s="3" t="str">
-        <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_LCD_BTN_3_UP) \</v>
-      </c>
-      <c r="W49" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_LCD_BTN_3_UP) \</v>
-      </c>
-      <c r="Y49" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_LCD_BTN_3_UP) \</v>
-      </c>
-      <c r="AA49" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_LCD_BTN_3_UP) \</v>
-      </c>
-      <c r="AC49" s="3" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_LCD_BTN_3_UP) \</v>
-      </c>
-      <c r="AE49" s="3" t="str">
-        <f t="shared" si="30"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_LCD_BTN_3_UP) \</v>
-      </c>
-    </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C13 PX_GPIO_LCD_BTN_3_UP</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>77</v>
       </c>
@@ -5511,31 +4443,11 @@
         <v>static const px_gpio_handle_t px_gpio_osc32_in = {PX_GPIO_OSC32_IN};</v>
       </c>
       <c r="U50" s="3" t="str">
-        <f t="shared" si="24"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_OSC32_IN) \</v>
-      </c>
-      <c r="W50" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_OSC32_IN) \</v>
-      </c>
-      <c r="Y50" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_OSC32_IN) \</v>
-      </c>
-      <c r="AA50" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_OSC32_IN) \</v>
-      </c>
-      <c r="AC50" s="3" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_OSC32_IN) \</v>
-      </c>
-      <c r="AE50" s="3" t="str">
-        <f t="shared" si="30"/>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_OSC32_IN) \</v>
-      </c>
-    </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C14 PX_GPIO_OSC32_IN</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>78</v>
       </c>
@@ -5597,31 +4509,11 @@
         <v>static const px_gpio_handle_t px_gpio_osc32_out = {PX_GPIO_OSC32_OUT};</v>
       </c>
       <c r="U51" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_MODER_INIT(",$A51,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_OSC32_OUT)</v>
-      </c>
-      <c r="W51" s="3" t="str">
-        <f t="shared" ref="W51" si="31">CONCATENATE("    + PX_GPIO_REG_OTYPER_INIT(",$A51,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_OSC32_OUT)</v>
-      </c>
-      <c r="Y51" s="3" t="str">
-        <f t="shared" ref="Y51" si="32">CONCATENATE("    + PX_GPIO_REG_OSPEEDR_INIT(",$A51,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_OSC32_OUT)</v>
-      </c>
-      <c r="AA51" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_PUPDR_INIT(",$A51,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_OSC32_OUT)</v>
-      </c>
-      <c r="AC51" s="3" t="str">
-        <f t="shared" ref="AC51" si="33">CONCATENATE("  + PX_GPIO_REG_ODR_INIT(",$A51,")")</f>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_OSC32_OUT)</v>
-      </c>
-      <c r="AE51" s="3" t="str">
-        <f t="shared" ref="AE51" si="34">CONCATENATE("    + PX_GPIO_REG_AFRH_INIT(",$A51,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRH_INIT(PX_GPIO_OSC32_OUT)</v>
-      </c>
-    </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C15 PX_GPIO_OSC32_OUT</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -5638,26 +4530,8 @@
       <c r="N52" s="9"/>
       <c r="O52" s="10"/>
       <c r="P52" s="2"/>
-      <c r="U52" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="W52" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y52" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AA52" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC52" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AE52" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>81</v>
       </c>
@@ -5719,31 +4593,11 @@
         <v>static const px_gpio_handle_t px_gpio_spi1_cs_sd = {PX_GPIO_SPI1_CS_SD};</v>
       </c>
       <c r="U53" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_MODER_INIT(",$A53,")")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_MODER_INIT(PX_GPIO_SPI1_CS_SD)</v>
-      </c>
-      <c r="W53" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_OTYPER_INIT(",$A53,")")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_OTYPER_INIT(PX_GPIO_SPI1_CS_SD)</v>
-      </c>
-      <c r="Y53" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_OSPEEDR_INIT(",$A53,")")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_SPI1_CS_SD)</v>
-      </c>
-      <c r="AA53" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_PUPDR_INIT(",$A53,")")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_PUPDR_INIT(PX_GPIO_SPI1_CS_SD)</v>
-      </c>
-      <c r="AC53" s="3" t="str">
-        <f>CONCATENATE("    PX_GPIO_REG_ODR_INIT(",$A53,")")</f>
-        <v xml:space="preserve">    PX_GPIO_REG_ODR_INIT(PX_GPIO_SPI1_CS_SD)</v>
-      </c>
-      <c r="AE53" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_AFRL_INIT(",$A53,")")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_AFRL_INIT(PX_GPIO_SPI1_CS_SD)</v>
-      </c>
-    </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_D2 PX_GPIO_SPI1_CS_SD</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="9"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
@@ -5760,26 +4614,8 @@
       <c r="N54" s="9"/>
       <c r="O54" s="10"/>
       <c r="P54" s="2"/>
-      <c r="U54" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="W54" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y54" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA54" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC54" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AE54" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>65</v>
       </c>
@@ -5841,31 +4677,11 @@
         <v>static const px_gpio_handle_t px_gpio_usr_led = {PX_GPIO_USR_LED};</v>
       </c>
       <c r="U55" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_MODER_INIT(",$A55,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_MODER_INIT(PX_GPIO_USR_LED) \</v>
-      </c>
-      <c r="W55" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_OTYPER_INIT(",$A55,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_OTYPER_INIT(PX_GPIO_USR_LED) \</v>
-      </c>
-      <c r="Y55" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_OSPEEDR_INIT(",$A55,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_USR_LED) \</v>
-      </c>
-      <c r="AA55" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_PUPDR_INIT(",$A55,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_PUPDR_INIT(PX_GPIO_USR_LED) \</v>
-      </c>
-      <c r="AC55" s="3" t="str">
-        <f>CONCATENATE("    PX_GPIO_REG_ODR_INIT(",$A55,") \")</f>
-        <v xml:space="preserve">    PX_GPIO_REG_ODR_INIT(PX_GPIO_USR_LED) \</v>
-      </c>
-      <c r="AE55" s="3" t="str">
-        <f>CONCATENATE("      PX_GPIO_REG_AFRL_INIT(",$A55,") \")</f>
-        <v xml:space="preserve">      PX_GPIO_REG_AFRL_INIT(PX_GPIO_USR_LED) \</v>
-      </c>
-    </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_H0 PX_GPIO_USR_LED</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>82</v>
       </c>
@@ -5927,31 +4743,11 @@
         <v>static const px_gpio_handle_t px_gpio_lcd_btn_2_rt = {PX_GPIO_LCD_BTN_2_RT};</v>
       </c>
       <c r="U56" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_MODER_INIT(",$A56,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_MODER_INIT(PX_GPIO_LCD_BTN_2_RT)</v>
-      </c>
-      <c r="W56" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_OTYPER_INIT(",$A56,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OTYPER_INIT(PX_GPIO_LCD_BTN_2_RT)</v>
-      </c>
-      <c r="Y56" s="3" t="str">
-        <f t="shared" ref="Y56" si="35">CONCATENATE("    + PX_GPIO_REG_OSPEEDR_INIT(",$A56,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_OSPEEDR_INIT(PX_GPIO_LCD_BTN_2_RT)</v>
-      </c>
-      <c r="AA56" s="3" t="str">
-        <f>CONCATENATE("    + PX_GPIO_REG_PUPDR_INIT(",$A56,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_PUPDR_INIT(PX_GPIO_LCD_BTN_2_RT)</v>
-      </c>
-      <c r="AC56" s="3" t="str">
-        <f t="shared" ref="AC56" si="36">CONCATENATE("  + PX_GPIO_REG_ODR_INIT(",$A56,")")</f>
-        <v xml:space="preserve">  + PX_GPIO_REG_ODR_INIT(PX_GPIO_LCD_BTN_2_RT)</v>
-      </c>
-      <c r="AE56" s="3" t="str">
-        <f t="shared" ref="AE56" si="37">CONCATENATE("    + PX_GPIO_REG_AFRL_INIT(",$A56,")")</f>
-        <v xml:space="preserve">    + PX_GPIO_REG_AFRL_INIT(PX_GPIO_LCD_BTN_2_RT)</v>
-      </c>
-    </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.2">
+        <f t="shared" ref="U56" si="3">CONCATENATE("#define PX_GPIO_",$B56,$C56," ",$A56)</f>
+        <v>#define PX_GPIO_H1 PX_GPIO_LCD_BTN_2_RT</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>

</xml_diff>